<commit_message>
Minor edits to lab 1. First push for lab 3 - task 1 complete.
</commit_message>
<xml_diff>
--- a/files/AzureDiscoveryDay-AnalyticsWithNRTIntelligence.xlsx
+++ b/files/AzureDiscoveryDay-AnalyticsWithNRTIntelligence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paelaz\Code\plzm.github\azure-discoveryday2019-mdw\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paelaz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69C1D5-0B0B-4014-AA54-6E31866A112B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080EA6A3-806A-4D4F-A805-2C0591B278E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19980" windowHeight="13215" xr2:uid="{7BACF9CF-52C3-4D9E-BD3F-2561D8743B78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="11775" xr2:uid="{7BACF9CF-52C3-4D9E-BD3F-2561D8743B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Session Name:</t>
   </si>
@@ -89,16 +89,7 @@
     <t>12:00 - 1:00PM</t>
   </si>
   <si>
-    <t>Data architects, engineers, and scientists - and anyone else interested in learning and building a modern data warehouse with hot and cold paths.</t>
-  </si>
-  <si>
-    <t>The modern data warehouse combines data storage, processing, and serving - and adds advanced analytics and stream processing capabilities to provide a single data estate with descriptive, predictive, and real-time aspects. This session dives deep into those areas while exploring modern techniques and Azure services to deliver a modern data estate.</t>
-  </si>
-  <si>
     <t>Azure Storage, Azure SQL DB, Azure Data Factory, Azure Databricks, Power BI, Event Hubs, Azure Functions, Azure Cognitive Services, and Azure Stream Analytics</t>
-  </si>
-  <si>
-    <t>Lab Pre-Requisites; Session Presentation</t>
   </si>
   <si>
     <t>Lunch</t>
@@ -121,15 +112,21 @@
     <t>Data Analytics &amp; NRT Intelligence with Azure</t>
   </si>
   <si>
-    <t>Learn about a modern data warehouse architecture and Azure technologies available to deliver that architecture.
-Get hands-on to build an end-to-end implementation with hot and cold paths using Azure data and AI technologies.</t>
-  </si>
-  <si>
     <t>Azure subscription with ability to roll out short-lived deployments of various Azure data technologies (or azure.com/free)
 We will cover lab pre-requisites at the start of the day so attendees can work on them (if needed) during the initial education session.</t>
   </si>
   <si>
-    <t>s</t>
+    <t>The modern data estate combines data storage, processing, and serving - and adds advanced analytics and stream processing capabilities to provide descriptive, predictive, and real-time aspects. This session covers those areas, and explores technologies and capabilities in each area to deliver a modern data estate on Azure.</t>
+  </si>
+  <si>
+    <t>Learn about a modern data estate architecture and Azure technologies available to deliver that architecture.
+Get hands-on to build an end-to-end implementation with hot and cold paths using Azure data and analytics technologies.</t>
+  </si>
+  <si>
+    <t>Data architects, engineers, and scientists as well as developers and other technologists interested in learning and building a modern data estate on Azure.</t>
+  </si>
+  <si>
+    <t>Session Presentation</t>
   </si>
 </sst>
 </file>
@@ -757,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73E2794-61EB-458A-83F5-E28BA65B12F7}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -818,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -933,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1063,7 +1060,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -1080,7 +1077,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="13"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1098,7 +1095,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="13"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1116,7 +1113,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="13"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1134,7 +1131,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="13"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1152,7 +1149,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="13"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1170,7 +1167,7 @@
       <c r="O21" s="12"/>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1188,12 +1185,12 @@
       <c r="O22" s="9"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1210,7 +1207,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="13"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1228,7 +1225,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1246,7 +1243,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="13"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1264,7 +1261,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1282,7 +1279,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1300,7 +1297,7 @@
       <c r="O28" s="12"/>
       <c r="P28" s="13"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1318,12 +1315,12 @@
       <c r="O29" s="9"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -1340,7 +1337,7 @@
       <c r="O30" s="12"/>
       <c r="P30" s="13"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1358,7 +1355,7 @@
       <c r="O31" s="12"/>
       <c r="P31" s="13"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1375,9 +1372,6 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
       <c r="P32" s="13"/>
-      <c r="S32" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -1521,7 +1515,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
@@ -1565,7 +1559,7 @@
         <v>17</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
@@ -1587,7 +1581,7 @@
         <v>18</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
@@ -1606,10 +1600,10 @@
     <row r="44" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>27</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
@@ -1628,7 +1622,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>15</v>
@@ -1704,6 +1698,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="36984313-f623-41bb-a65c-16a37d29f6f8" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1712,9 +1716,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B38F4F3D64ED8742A4722C7FA5D444DB" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eea62de22946d39945f4b56eb92f81ad">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36984313-f623-41bb-a65c-16a37d29f6f8" xmlns:ns3="fa40b356-8329-45cf-bdd1-8a6639dbec32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="826e6c641157ccfc2a59418abe647b4a" ns2:_="" ns3:_="">
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B38F4F3D64ED8742A4722C7FA5D444DB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6af96e04080b60a45b019feeca7a37aa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="36984313-f623-41bb-a65c-16a37d29f6f8" xmlns:ns3="fa40b356-8329-45cf-bdd1-8a6639dbec32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a16216aa0538460924a13a680e0634d6" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="36984313-f623-41bb-a65c-16a37d29f6f8"/>
     <xsd:import namespace="fa40b356-8329-45cf-bdd1-8a6639dbec32"/>
     <xsd:element name="properties">
@@ -1729,11 +1734,29 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="16" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="17" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="36984313-f623-41bb-a65c-16a37d29f6f8" elementFormDefault="qualified">
@@ -1755,6 +1778,18 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="false">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -1891,40 +1926,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D93BE2C-4E24-4969-8FC9-BEB174790CF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1388E25D-DC5B-4237-A6F6-BCA44DCF443F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="36984313-f623-41bb-a65c-16a37d29f6f8"/>
-    <ds:schemaRef ds:uri="fa40b356-8329-45cf-bdd1-8a6639dbec32"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9F3368-7CCA-4DBB-9695-AFCE59563191}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1937,6 +1939,35 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="fa40b356-8329-45cf-bdd1-8a6639dbec32"/>
     <ds:schemaRef ds:uri="36984313-f623-41bb-a65c-16a37d29f6f8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D93BE2C-4E24-4969-8FC9-BEB174790CF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E98CEAB1-77ED-4214-BDBE-7E2B97AA29FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="36984313-f623-41bb-a65c-16a37d29f6f8"/>
+    <ds:schemaRef ds:uri="fa40b356-8329-45cf-bdd1-8a6639dbec32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>